<commit_message>
Update lit_review_data - Frantisek.xlsx
</commit_message>
<xml_diff>
--- a/data/lit_review_data - Frantisek.xlsx
+++ b/data/lit_review_data - Frantisek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Papers-GitHub\SimPsychReview\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4D93D3-C183-447D-AADB-9921F4A48E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9D4E43-318C-4D21-9BDF-B1179A0596B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="3540" windowWidth="21810" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_sim" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1685" uniqueCount="297">
   <si>
     <t>year</t>
   </si>
@@ -810,9 +810,6 @@
     <t>"The outcome variables are CI coverage rates for model parameters and rejection rates for a test of correct model specification." (p. 553)</t>
   </si>
   <si>
-    <t>large: sem model with multiple indicators etc</t>
-  </si>
-  <si>
     <t>relative bias, absolute relative bias</t>
   </si>
   <si>
@@ -924,9 +921,6 @@
     <t>not applicable</t>
   </si>
   <si>
-    <t>anticlustering solutions</t>
-  </si>
-  <si>
     <t>anticluster editing objective</t>
   </si>
   <si>
@@ -958,9 +952,6 @@
     <t>"For the simulation, it is hypothesized that classification accuracy across models would increase as sample size, number of item categories, number of items, prevalence of the diagnosis, and the diagnosis-test correlation increase." (p. 241)</t>
   </si>
   <si>
-    <t>classification</t>
-  </si>
-  <si>
     <t>accuracy, sensitivity, specificity, classification rate</t>
   </si>
   <si>
@@ -974,9 +965,6 @@
   </si>
   <si>
     <t>"This subsection describes the effects on test linking accuracy of varying distributions of examinee ability and characteristics of raters and tasks for a new test." (p. 1444)</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Java</t>
@@ -1041,6 +1029,12 @@
   <si>
     <t>https://doi.org/10.3758/s13428-021-01634-1</t>
   </si>
+  <si>
+    <t>"The goal of the simulation was to create different arrays for three numerosities (5, 10, 20 elements), keeping constant the convex hull (controlled at 150000 pixels) and the total area (controlled at 20000 pixels) across quantities" (p. 153)</t>
+  </si>
+  <si>
+    <t>"it specifically focused on how the identification constraint influences the information criteria" (p. 797)</t>
+  </si>
 </sst>
 </file>
 
@@ -1050,7 +1044,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="d\-m"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1090,19 +1084,20 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1114,30 +1109,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1356,39 +1355,48 @@
   </sheetPr>
   <dimension ref="A1:BB1161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="8" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" customWidth="1"/>
-    <col min="13" max="13" width="15.7109375" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" customWidth="1"/>
-    <col min="17" max="17" width="15.85546875" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" customWidth="1"/>
-    <col min="20" max="21" width="17.42578125" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" customWidth="1"/>
-    <col min="27" max="27" width="18.140625" customWidth="1"/>
-    <col min="32" max="32" width="13.85546875" customWidth="1"/>
-    <col min="39" max="39" width="15.42578125" customWidth="1"/>
-    <col min="42" max="42" width="16.140625" customWidth="1"/>
-    <col min="43" max="43" width="13.28515625" customWidth="1"/>
-    <col min="44" max="44" width="15.7109375" customWidth="1"/>
-    <col min="45" max="45" width="17.42578125" customWidth="1"/>
-    <col min="46" max="47" width="15.7109375" customWidth="1"/>
-    <col min="48" max="48" width="15.140625" customWidth="1"/>
-    <col min="49" max="49" width="18.42578125" customWidth="1"/>
-    <col min="50" max="54" width="15.28515625" customWidth="1"/>
+    <col min="1" max="2" width="12.5546875" style="2"/>
+    <col min="3" max="3" width="9" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" style="2"/>
+    <col min="8" max="9" width="14.44140625" style="2" customWidth="1"/>
+    <col min="10" max="11" width="14.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.6640625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" style="2"/>
+    <col min="15" max="15" width="14.88671875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="13.88671875" style="2" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" style="2" customWidth="1"/>
+    <col min="18" max="18" width="12.5546875" style="2"/>
+    <col min="19" max="19" width="15.33203125" style="2" customWidth="1"/>
+    <col min="20" max="21" width="17.44140625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="14.44140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="18.109375" style="2" customWidth="1"/>
+    <col min="24" max="26" width="12.5546875" style="2"/>
+    <col min="27" max="27" width="18.109375" style="2" customWidth="1"/>
+    <col min="28" max="31" width="12.5546875" style="2"/>
+    <col min="32" max="32" width="13.88671875" style="2" customWidth="1"/>
+    <col min="33" max="38" width="12.5546875" style="2"/>
+    <col min="39" max="39" width="15.44140625" style="2" customWidth="1"/>
+    <col min="40" max="41" width="12.5546875" style="2"/>
+    <col min="42" max="42" width="16.109375" style="2" customWidth="1"/>
+    <col min="43" max="43" width="13.33203125" style="2" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" style="2" customWidth="1"/>
+    <col min="45" max="45" width="17.44140625" style="2" customWidth="1"/>
+    <col min="46" max="47" width="15.6640625" style="2" customWidth="1"/>
+    <col min="48" max="48" width="15.109375" style="2" customWidth="1"/>
+    <col min="49" max="49" width="18.44140625" style="2" customWidth="1"/>
+    <col min="50" max="54" width="15.33203125" style="2" customWidth="1"/>
+    <col min="55" max="16384" width="12.5546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:54">
@@ -1563,7 +1571,7 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1619,9 +1627,9 @@
       <c r="AW2" s="1"/>
       <c r="AX2" s="1"/>
       <c r="AY2" s="1"/>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3">
+      <c r="AZ2" s="4"/>
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="4">
         <v>45082</v>
       </c>
     </row>
@@ -1635,7 +1643,7 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -1756,7 +1764,7 @@
       <c r="AT3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU3" s="2" t="s">
+      <c r="AU3" s="3" t="s">
         <v>71</v>
       </c>
       <c r="AV3" s="1" t="s">
@@ -1765,17 +1773,17 @@
       <c r="AW3" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AX3" s="4" t="s">
+      <c r="AX3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AY3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AZ3" s="3"/>
+      <c r="AZ3" s="4"/>
       <c r="BA3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB3" s="3">
+      <c r="BB3" s="4">
         <v>45082</v>
       </c>
     </row>
@@ -1789,7 +1797,7 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -1921,11 +1929,11 @@
       <c r="AY4" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AZ4" s="3"/>
+      <c r="AZ4" s="4"/>
       <c r="BA4" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BB4" s="4">
         <v>45082</v>
       </c>
     </row>
@@ -1939,7 +1947,7 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1996,8 +2004,8 @@
       <c r="AX5" s="1"/>
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
-      <c r="BA5" s="3"/>
-      <c r="BB5" s="3">
+      <c r="BA5" s="4"/>
+      <c r="BB5" s="4">
         <v>45082</v>
       </c>
     </row>
@@ -2011,7 +2019,7 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>86</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -2149,7 +2157,7 @@
       <c r="BA6" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BB6" s="3">
+      <c r="BB6" s="4">
         <v>45082</v>
       </c>
     </row>
@@ -2163,7 +2171,7 @@
       <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -2220,8 +2228,8 @@
       <c r="AX7" s="1"/>
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
-      <c r="BA7" s="3"/>
-      <c r="BB7" s="3">
+      <c r="BA7" s="4"/>
+      <c r="BB7" s="4">
         <v>45082</v>
       </c>
     </row>
@@ -2235,7 +2243,7 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>94</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -2292,8 +2300,8 @@
       <c r="AX8" s="1"/>
       <c r="AY8" s="1"/>
       <c r="AZ8" s="1"/>
-      <c r="BA8" s="3"/>
-      <c r="BB8" s="3">
+      <c r="BA8" s="4"/>
+      <c r="BB8" s="4">
         <v>45082</v>
       </c>
     </row>
@@ -2304,10 +2312,10 @@
       <c r="B9" s="1">
         <v>2022</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>44987</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -2399,7 +2407,7 @@
         <v>59</v>
       </c>
       <c r="AK9" s="1"/>
-      <c r="AL9" s="7" t="s">
+      <c r="AL9" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM9" s="1" t="s">
@@ -2441,7 +2449,7 @@
       <c r="BA9" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB9" s="3">
+      <c r="BB9" s="4">
         <v>45096</v>
       </c>
     </row>
@@ -2452,10 +2460,10 @@
       <c r="B10" s="1">
         <v>2022</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>44987</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>103</v>
       </c>
       <c r="E10" s="1" t="s">
@@ -2547,7 +2555,7 @@
         <v>59</v>
       </c>
       <c r="AK10" s="1"/>
-      <c r="AL10" s="7" t="s">
+      <c r="AL10" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM10" s="1" t="s">
@@ -2585,7 +2593,7 @@
       <c r="BA10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB10" s="3">
+      <c r="BB10" s="4">
         <v>45096</v>
       </c>
     </row>
@@ -2596,10 +2604,10 @@
       <c r="B11" s="1">
         <v>2022</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>44987</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>107</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2666,10 +2674,10 @@
       <c r="B12" s="1">
         <v>2022</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>44987</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>108</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2763,7 +2771,7 @@
         <v>59</v>
       </c>
       <c r="AK12" s="1"/>
-      <c r="AL12" s="7" t="s">
+      <c r="AL12" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM12" s="1" t="s">
@@ -2788,7 +2796,7 @@
       <c r="AT12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU12" s="5" t="s">
+      <c r="AU12" s="6" t="s">
         <v>110</v>
       </c>
       <c r="AV12" s="1" t="s">
@@ -2805,7 +2813,7 @@
       <c r="BA12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB12" s="3">
+      <c r="BB12" s="4">
         <v>45105</v>
       </c>
     </row>
@@ -2816,10 +2824,10 @@
       <c r="B13" s="1">
         <v>2022</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>44987</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>111</v>
       </c>
       <c r="E13" s="1" t="s">
@@ -2913,7 +2921,7 @@
         <v>59</v>
       </c>
       <c r="AK13" s="1"/>
-      <c r="AL13" s="7" t="s">
+      <c r="AL13" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM13" s="1" t="s">
@@ -2951,7 +2959,7 @@
       <c r="BA13" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB13" s="3">
+      <c r="BB13" s="4">
         <v>45105</v>
       </c>
     </row>
@@ -2962,10 +2970,10 @@
       <c r="B14" s="1">
         <v>2022</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="7">
         <v>44987</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>114</v>
       </c>
       <c r="E14" s="1" t="s">
@@ -3059,7 +3067,7 @@
         <v>59</v>
       </c>
       <c r="AK14" s="1"/>
-      <c r="AL14" s="7" t="s">
+      <c r="AL14" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM14" s="1" t="s">
@@ -3097,7 +3105,7 @@
       <c r="BA14" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB14" s="3">
+      <c r="BB14" s="4">
         <v>45105</v>
       </c>
     </row>
@@ -3108,10 +3116,10 @@
       <c r="B15" s="1">
         <v>2022</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="7">
         <v>44987</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>117</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -3203,7 +3211,7 @@
         <v>59</v>
       </c>
       <c r="AK15" s="1"/>
-      <c r="AL15" s="7" t="s">
+      <c r="AL15" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM15" s="1" t="s">
@@ -3243,7 +3251,7 @@
       <c r="BA15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB15" s="3">
+      <c r="BB15" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -3254,10 +3262,10 @@
       <c r="B16" s="1">
         <v>2022</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="7">
         <v>44987</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>121</v>
       </c>
       <c r="E16" s="1" t="s">
@@ -3351,7 +3359,7 @@
         <v>59</v>
       </c>
       <c r="AK16" s="1"/>
-      <c r="AL16" s="7" t="s">
+      <c r="AL16" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM16" s="1" t="s">
@@ -3376,7 +3384,7 @@
       <c r="AT16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU16" s="2" t="s">
+      <c r="AU16" s="3" t="s">
         <v>125</v>
       </c>
       <c r="AV16" s="1" t="s">
@@ -3393,7 +3401,7 @@
       <c r="BA16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB16" s="3">
+      <c r="BB16" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -3404,10 +3412,10 @@
       <c r="B17" s="1">
         <v>2022</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="7">
         <v>44987</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>126</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -3501,7 +3509,7 @@
         <v>59</v>
       </c>
       <c r="AK17" s="1"/>
-      <c r="AL17" s="7" t="s">
+      <c r="AL17" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM17" s="1" t="s">
@@ -3543,7 +3551,7 @@
       <c r="BA17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB17" s="3">
+      <c r="BB17" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -3554,10 +3562,10 @@
       <c r="B18" s="1">
         <v>2022</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="7">
         <v>44987</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>134</v>
       </c>
       <c r="E18" s="1" t="s">
@@ -3691,7 +3699,7 @@
       <c r="BA18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB18" s="3">
+      <c r="BB18" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -3702,10 +3710,10 @@
       <c r="B19" s="1">
         <v>2022</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
         <v>44987</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>141</v>
       </c>
       <c r="E19" s="1" t="s">
@@ -3801,7 +3809,7 @@
         <v>59</v>
       </c>
       <c r="AK19" s="1"/>
-      <c r="AL19" s="7" t="s">
+      <c r="AL19" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM19" s="1" t="s">
@@ -3839,7 +3847,7 @@
       <c r="BA19" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB19" s="3">
+      <c r="BB19" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -3850,10 +3858,10 @@
       <c r="B20" s="1">
         <v>2022</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="7">
         <v>44987</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>144</v>
       </c>
       <c r="E20" s="1" t="s">
@@ -3947,7 +3955,7 @@
         <v>59</v>
       </c>
       <c r="AK20" s="1"/>
-      <c r="AL20" s="7" t="s">
+      <c r="AL20" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM20" s="1" t="s">
@@ -3987,7 +3995,7 @@
       <c r="BA20" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB20" s="3">
+      <c r="BB20" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -3998,10 +4006,10 @@
       <c r="B21" s="1">
         <v>2022</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="7">
         <v>44987</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>148</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -4093,7 +4101,7 @@
         <v>59</v>
       </c>
       <c r="AK21" s="1"/>
-      <c r="AL21" s="7" t="s">
+      <c r="AL21" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM21" s="1" t="s">
@@ -4131,7 +4139,7 @@
       <c r="BA21" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB21" s="3">
+      <c r="BB21" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -4142,10 +4150,10 @@
       <c r="B22" s="1">
         <v>2022</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="7">
         <v>44987</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>150</v>
       </c>
       <c r="E22" s="1" t="s">
@@ -4241,7 +4249,7 @@
         <v>59</v>
       </c>
       <c r="AK22" s="1"/>
-      <c r="AL22" s="7" t="s">
+      <c r="AL22" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM22" s="1" t="s">
@@ -4266,7 +4274,7 @@
       <c r="AT22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU22" s="5" t="s">
+      <c r="AU22" s="6" t="s">
         <v>154</v>
       </c>
       <c r="AV22" s="1" t="s">
@@ -4283,7 +4291,7 @@
       <c r="BA22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB22" s="3">
+      <c r="BB22" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -4294,10 +4302,10 @@
       <c r="B23" s="1">
         <v>2022</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="7">
         <v>44987</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>155</v>
       </c>
       <c r="E23" s="1" t="s">
@@ -4364,10 +4372,10 @@
       <c r="B24" s="1">
         <v>2022</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="7">
         <v>44987</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>156</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -4463,7 +4471,7 @@
         <v>59</v>
       </c>
       <c r="AK24" s="1"/>
-      <c r="AL24" s="7" t="s">
+      <c r="AL24" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM24" s="1" t="s">
@@ -4501,7 +4509,7 @@
       <c r="BA24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB24" s="3">
+      <c r="BB24" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -4512,10 +4520,10 @@
       <c r="B25" s="1">
         <v>2022</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="7">
         <v>44987</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>159</v>
       </c>
       <c r="E25" s="1" t="s">
@@ -4607,7 +4615,7 @@
         <v>59</v>
       </c>
       <c r="AK25" s="1"/>
-      <c r="AL25" s="7" t="s">
+      <c r="AL25" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM25" s="1" t="s">
@@ -4632,7 +4640,7 @@
       <c r="AT25" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU25" s="5" t="s">
+      <c r="AU25" s="6" t="s">
         <v>161</v>
       </c>
       <c r="AV25" s="1" t="s">
@@ -4649,7 +4657,7 @@
       <c r="BA25" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB25" s="3">
+      <c r="BB25" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -4663,7 +4671,7 @@
       <c r="C26" s="1">
         <v>3</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>162</v>
       </c>
       <c r="E26" s="1" t="s">
@@ -4685,7 +4693,7 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="8"/>
+      <c r="R26" s="9"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
@@ -4733,7 +4741,7 @@
       <c r="C27" s="1">
         <v>3</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>164</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -4780,7 +4788,9 @@
       <c r="T27" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="U27" s="1"/>
+      <c r="U27" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="V27" s="1">
         <v>6</v>
       </c>
@@ -4827,7 +4837,7 @@
         <v>59</v>
       </c>
       <c r="AK27" s="1"/>
-      <c r="AL27" s="7" t="s">
+      <c r="AL27" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM27" s="1" t="s">
@@ -4852,7 +4862,7 @@
       <c r="AT27" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU27" s="5" t="s">
+      <c r="AU27" s="6" t="s">
         <v>168</v>
       </c>
       <c r="AV27" s="1" t="s">
@@ -4869,7 +4879,7 @@
       <c r="BA27" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB27" s="3">
+      <c r="BB27" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -4883,7 +4893,7 @@
       <c r="C28" s="1">
         <v>3</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="3" t="s">
         <v>169</v>
       </c>
       <c r="E28" s="1" t="s">
@@ -4953,7 +4963,7 @@
       <c r="C29" s="1">
         <v>3</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>170</v>
       </c>
       <c r="E29" s="1" t="s">
@@ -5023,7 +5033,7 @@
       <c r="C30" s="1">
         <v>3</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="6" t="s">
         <v>171</v>
       </c>
       <c r="E30" s="1" t="s">
@@ -5093,7 +5103,7 @@
       <c r="C31" s="1">
         <v>3</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="6" t="s">
         <v>172</v>
       </c>
       <c r="E31" s="1" t="s">
@@ -5189,7 +5199,7 @@
         <v>81</v>
       </c>
       <c r="AK31" s="1"/>
-      <c r="AL31" s="7" t="s">
+      <c r="AL31" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM31" s="1" t="s">
@@ -5229,7 +5239,7 @@
       <c r="BA31" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB31" s="3">
+      <c r="BB31" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -5243,7 +5253,7 @@
       <c r="C32" s="1">
         <v>3</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>176</v>
       </c>
       <c r="E32" s="1" t="s">
@@ -5313,7 +5323,7 @@
       <c r="C33" s="1">
         <v>3</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>177</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -5383,7 +5393,7 @@
       <c r="C34" s="1">
         <v>3</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>178</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -5477,7 +5487,7 @@
         <v>59</v>
       </c>
       <c r="AK34" s="1"/>
-      <c r="AL34" s="7" t="s">
+      <c r="AL34" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM34" s="1" t="s">
@@ -5502,7 +5512,7 @@
       <c r="AT34" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AU34" s="5" t="s">
+      <c r="AU34" s="6" t="s">
         <v>180</v>
       </c>
       <c r="AV34" s="1"/>
@@ -5519,7 +5529,7 @@
       <c r="BA34" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB34" s="3">
+      <c r="BB34" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -5533,7 +5543,7 @@
       <c r="C35" s="1">
         <v>3</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>182</v>
       </c>
       <c r="E35" s="1" t="s">
@@ -5603,7 +5613,7 @@
       <c r="C36" s="1">
         <v>3</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>183</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -5673,7 +5683,7 @@
       <c r="C37" s="1">
         <v>3</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>184</v>
       </c>
       <c r="E37" s="1" t="s">
@@ -5743,7 +5753,7 @@
       <c r="C38" s="1">
         <v>3</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>185</v>
       </c>
       <c r="E38" s="1" t="s">
@@ -5813,7 +5823,7 @@
       <c r="C39" s="1">
         <v>3</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>186</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -5883,7 +5893,7 @@
       <c r="C40" s="1">
         <v>3</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="6" t="s">
         <v>187</v>
       </c>
       <c r="E40" s="1" t="s">
@@ -5977,7 +5987,7 @@
         <v>59</v>
       </c>
       <c r="AK40" s="1"/>
-      <c r="AL40" s="7" t="s">
+      <c r="AL40" s="8" t="s">
         <v>68</v>
       </c>
       <c r="AM40" s="1" t="s">
@@ -6017,7 +6027,7 @@
       <c r="BA40" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB40" s="3">
+      <c r="BB40" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -6031,7 +6041,7 @@
       <c r="C41" s="1">
         <v>3</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="6" t="s">
         <v>191</v>
       </c>
       <c r="E41" s="1" t="s">
@@ -6101,7 +6111,7 @@
       <c r="C42" s="1">
         <v>3</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="6" t="s">
         <v>192</v>
       </c>
       <c r="E42" s="1" t="s">
@@ -6171,7 +6181,7 @@
       <c r="C43" s="1">
         <v>3</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="6" t="s">
         <v>193</v>
       </c>
       <c r="E43" s="1" t="s">
@@ -6241,7 +6251,7 @@
       <c r="C44" s="1">
         <v>3</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="6" t="s">
         <v>194</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -6311,7 +6321,7 @@
       <c r="C45" s="1">
         <v>3</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="6" t="s">
         <v>195</v>
       </c>
       <c r="E45" s="1" t="s">
@@ -6381,7 +6391,7 @@
       <c r="C46" s="1">
         <v>3</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="6" t="s">
         <v>196</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -6451,7 +6461,7 @@
       <c r="C47" s="1">
         <v>3</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="6" t="s">
         <v>197</v>
       </c>
       <c r="E47" s="1" t="s">
@@ -6521,7 +6531,7 @@
       <c r="C48" s="1">
         <v>3</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="6" t="s">
         <v>198</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -6591,7 +6601,7 @@
       <c r="C49" s="1">
         <v>3</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="6" t="s">
         <v>199</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -6661,7 +6671,7 @@
       <c r="C50" s="1">
         <v>3</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="6" t="s">
         <v>200</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -6731,7 +6741,7 @@
       <c r="C51" s="1">
         <v>3</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="6" t="s">
         <v>201</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -6801,7 +6811,7 @@
       <c r="C52" s="1">
         <v>3</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="6" t="s">
         <v>202</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -6937,7 +6947,7 @@
       <c r="BA52" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BB52" s="3">
+      <c r="BB52" s="4">
         <v>45106</v>
       </c>
     </row>
@@ -6951,7 +6961,7 @@
       <c r="C53" s="1">
         <v>3</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="6" t="s">
         <v>207</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -7021,7 +7031,7 @@
       <c r="C54" s="1">
         <v>3</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="6" t="s">
         <v>208</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -7091,7 +7101,7 @@
       <c r="C55" s="1">
         <v>3</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D55" s="3" t="s">
         <v>209</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -7161,7 +7171,7 @@
       <c r="C56" s="1">
         <v>4</v>
       </c>
-      <c r="D56" s="2" t="s">
+      <c r="D56" s="3" t="s">
         <v>210</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -7231,7 +7241,7 @@
       <c r="C57" s="1">
         <v>4</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="6" t="s">
         <v>211</v>
       </c>
       <c r="E57" s="1" t="s">
@@ -7296,19 +7306,19 @@
       <c r="Z57" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="AA57" s="9" t="s">
+      <c r="AA57" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AB57" s="9" t="s">
+      <c r="AB57" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AC57" s="9" t="s">
+      <c r="AC57" s="10" t="s">
         <v>57</v>
       </c>
       <c r="AD57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AE57" s="9" t="s">
+      <c r="AE57" s="10" t="s">
         <v>57</v>
       </c>
       <c r="AF57" s="1" t="s">
@@ -7354,7 +7364,7 @@
       <c r="AT57" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU57" s="2" t="s">
+      <c r="AU57" s="3" t="s">
         <v>214</v>
       </c>
       <c r="AV57" s="1" t="s">
@@ -7371,7 +7381,7 @@
       <c r="BA57" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB57" s="3">
+      <c r="BB57" s="4">
         <v>45100</v>
       </c>
     </row>
@@ -7385,7 +7395,7 @@
       <c r="C58" s="1">
         <v>4</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="6" t="s">
         <v>215</v>
       </c>
       <c r="E58" s="1" t="s">
@@ -7516,10 +7526,10 @@
       </c>
       <c r="AY58" s="1"/>
       <c r="AZ58" s="1"/>
-      <c r="BA58" s="10" t="s">
+      <c r="BA58" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="BB58" s="11">
+      <c r="BB58" s="12">
         <v>45100</v>
       </c>
     </row>
@@ -7533,7 +7543,7 @@
       <c r="C59" s="1">
         <v>4</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="6" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="1" t="s">
@@ -7583,8 +7593,8 @@
       <c r="U59" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="V59" s="1" t="s">
-        <v>222</v>
+      <c r="V59" s="1">
+        <v>190</v>
       </c>
       <c r="W59" s="1" t="s">
         <v>59</v>
@@ -7623,7 +7633,7 @@
         <v>57</v>
       </c>
       <c r="AI59" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AJ59" s="1" t="s">
         <v>59</v>
@@ -7654,8 +7664,8 @@
       <c r="AT59" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU59" s="2" t="s">
-        <v>224</v>
+      <c r="AU59" s="3" t="s">
+        <v>223</v>
       </c>
       <c r="AV59" s="1" t="s">
         <v>59</v>
@@ -7668,10 +7678,10 @@
       </c>
       <c r="AY59" s="1"/>
       <c r="AZ59" s="1"/>
-      <c r="BA59" s="10" t="s">
+      <c r="BA59" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="BB59" s="11">
+      <c r="BB59" s="12">
         <v>45100</v>
       </c>
     </row>
@@ -7685,8 +7695,8 @@
       <c r="C60" s="1">
         <v>4</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>225</v>
+      <c r="D60" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>55</v>
@@ -7707,7 +7717,7 @@
         <v>59</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>61</v>
@@ -7748,7 +7758,7 @@
         <v>6</v>
       </c>
       <c r="Z60" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AA60" s="1" t="s">
         <v>59</v>
@@ -7806,8 +7816,8 @@
       <c r="AT60" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU60" s="5" t="s">
-        <v>228</v>
+      <c r="AU60" s="6" t="s">
+        <v>227</v>
       </c>
       <c r="AV60" s="1" t="s">
         <v>59</v>
@@ -7823,7 +7833,7 @@
       <c r="BA60" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB60" s="11">
+      <c r="BB60" s="12">
         <v>45100</v>
       </c>
     </row>
@@ -7837,8 +7847,8 @@
       <c r="C61" s="1">
         <v>4</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>229</v>
+      <c r="D61" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>55</v>
@@ -7907,8 +7917,8 @@
       <c r="C62" s="1">
         <v>4</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>230</v>
+      <c r="D62" s="3" t="s">
+        <v>229</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>55</v>
@@ -7977,8 +7987,8 @@
       <c r="C63" s="1">
         <v>4</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>231</v>
+      <c r="D63" s="6" t="s">
+        <v>230</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>55</v>
@@ -8047,8 +8057,8 @@
       <c r="C64" s="1">
         <v>4</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>232</v>
+      <c r="D64" s="6" t="s">
+        <v>231</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>55</v>
@@ -8069,7 +8079,7 @@
         <v>59</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L64" s="1" t="s">
         <v>61</v>
@@ -8137,7 +8147,7 @@
         <v>57</v>
       </c>
       <c r="AI64" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AJ64" s="1"/>
       <c r="AK64" s="1"/>
@@ -8166,8 +8176,8 @@
       <c r="AT64" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU64" s="2" t="s">
-        <v>235</v>
+      <c r="AU64" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="AV64" s="1" t="s">
         <v>59</v>
@@ -8183,7 +8193,7 @@
       <c r="BA64" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB64" s="11">
+      <c r="BB64" s="12">
         <v>45100</v>
       </c>
     </row>
@@ -8197,8 +8207,8 @@
       <c r="C65" s="1">
         <v>4</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>236</v>
+      <c r="D65" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>55</v>
@@ -8267,8 +8277,8 @@
       <c r="C66" s="1">
         <v>1</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>237</v>
+      <c r="D66" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>55</v>
@@ -8328,22 +8338,22 @@
       <c r="Z66" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AA66" s="9" t="s">
+      <c r="AA66" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AB66" s="9" t="s">
+      <c r="AB66" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AC66" s="9" t="s">
+      <c r="AC66" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AD66" s="9" t="s">
+      <c r="AD66" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AE66" s="9" t="s">
+      <c r="AE66" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AF66" s="9" t="s">
+      <c r="AF66" s="10" t="s">
         <v>57</v>
       </c>
       <c r="AG66" s="1" t="s">
@@ -8353,14 +8363,14 @@
         <v>57</v>
       </c>
       <c r="AI66" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AJ66" s="1" t="s">
         <v>59</v>
       </c>
       <c r="AK66" s="1"/>
       <c r="AL66" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AM66" s="1" t="s">
         <v>57</v>
@@ -8397,7 +8407,7 @@
       <c r="BA66" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB66" s="11">
+      <c r="BB66" s="12">
         <v>45107</v>
       </c>
     </row>
@@ -8411,8 +8421,8 @@
       <c r="C67" s="1">
         <v>1</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>240</v>
+      <c r="D67" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>55</v>
@@ -8431,7 +8441,7 @@
         <v>59</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>61</v>
@@ -8443,7 +8453,7 @@
         <v>1</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P67" s="1">
         <v>1</v>
@@ -8462,7 +8472,7 @@
         <v>59</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="W67" s="1" t="s">
         <v>57</v>
@@ -8501,7 +8511,7 @@
         <v>57</v>
       </c>
       <c r="AI67" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AJ67" s="1" t="s">
         <v>59</v>
@@ -8545,7 +8555,7 @@
       <c r="BA67" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB67" s="11">
+      <c r="BB67" s="12">
         <v>45107</v>
       </c>
     </row>
@@ -8559,8 +8569,8 @@
       <c r="C68" s="1">
         <v>1</v>
       </c>
-      <c r="D68" s="5" t="s">
-        <v>245</v>
+      <c r="D68" s="6" t="s">
+        <v>244</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>55</v>
@@ -8629,8 +8639,8 @@
       <c r="C69" s="1">
         <v>1</v>
       </c>
-      <c r="D69" s="2" t="s">
-        <v>246</v>
+      <c r="D69" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>55</v>
@@ -8699,8 +8709,8 @@
       <c r="C70" s="1">
         <v>1</v>
       </c>
-      <c r="D70" s="5" t="s">
-        <v>247</v>
+      <c r="D70" s="6" t="s">
+        <v>246</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>55</v>
@@ -8769,8 +8779,8 @@
       <c r="C71" s="1">
         <v>1</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>248</v>
+      <c r="D71" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>55</v>
@@ -8839,8 +8849,8 @@
       <c r="C72" s="1">
         <v>1</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>249</v>
+      <c r="D72" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>55</v>
@@ -8909,8 +8919,8 @@
       <c r="C73" s="1">
         <v>1</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>250</v>
+      <c r="D73" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>55</v>
@@ -8979,8 +8989,8 @@
       <c r="C74" s="1">
         <v>1</v>
       </c>
-      <c r="D74" s="5" t="s">
-        <v>251</v>
+      <c r="D74" s="6" t="s">
+        <v>250</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>55</v>
@@ -9049,8 +9059,8 @@
       <c r="C75" s="1">
         <v>2</v>
       </c>
-      <c r="D75" s="5" t="s">
-        <v>252</v>
+      <c r="D75" s="6" t="s">
+        <v>251</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>55</v>
@@ -9069,7 +9079,7 @@
         <v>59</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>61</v>
@@ -9094,7 +9104,7 @@
         <v>59</v>
       </c>
       <c r="T75" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="U75" s="1" t="s">
         <v>59</v>
@@ -9112,7 +9122,7 @@
         <v>63</v>
       </c>
       <c r="Z75" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AA75" s="1" t="s">
         <v>57</v>
@@ -9168,8 +9178,8 @@
       <c r="AT75" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU75" s="5" t="s">
-        <v>256</v>
+      <c r="AU75" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="AV75" s="1" t="s">
         <v>59</v>
@@ -9185,7 +9195,7 @@
       <c r="BA75" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB75" s="3">
+      <c r="BB75" s="4">
         <v>45110</v>
       </c>
     </row>
@@ -9199,8 +9209,8 @@
       <c r="C76" s="1">
         <v>2</v>
       </c>
-      <c r="D76" s="5" t="s">
-        <v>257</v>
+      <c r="D76" s="6" t="s">
+        <v>256</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>55</v>
@@ -9219,7 +9229,7 @@
         <v>59</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>61</v>
@@ -9245,22 +9255,22 @@
       </c>
       <c r="T76" s="1"/>
       <c r="U76" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="V76" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="W76" s="1" t="s">
         <v>57</v>
       </c>
       <c r="X76" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y76" s="1">
         <v>3</v>
       </c>
       <c r="Z76" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AA76" s="1" t="s">
         <v>57</v>
@@ -9287,7 +9297,7 @@
         <v>57</v>
       </c>
       <c r="AI76" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AJ76" s="1" t="s">
         <v>59</v>
@@ -9318,8 +9328,8 @@
       <c r="AT76" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU76" s="5" t="s">
-        <v>262</v>
+      <c r="AU76" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="AV76" s="1"/>
       <c r="AW76" s="1" t="s">
@@ -9330,12 +9340,12 @@
       </c>
       <c r="AY76" s="1"/>
       <c r="AZ76" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="BA76" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB76" s="3">
+      <c r="BB76" s="4">
         <v>45110</v>
       </c>
     </row>
@@ -9349,8 +9359,8 @@
       <c r="C77" s="1">
         <v>2</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>264</v>
+      <c r="D77" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>55</v>
@@ -9419,8 +9429,8 @@
       <c r="C78" s="1">
         <v>2</v>
       </c>
-      <c r="D78" s="5" t="s">
-        <v>265</v>
+      <c r="D78" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>55</v>
@@ -9489,8 +9499,8 @@
       <c r="C79" s="1">
         <v>2</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>266</v>
+      <c r="D79" s="3" t="s">
+        <v>264</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>55</v>
@@ -9511,7 +9521,7 @@
         <v>59</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>61</v>
@@ -9540,7 +9550,7 @@
         <v>59</v>
       </c>
       <c r="V79" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="W79" s="1" t="s">
         <v>59</v>
@@ -9621,7 +9631,7 @@
       <c r="BA79" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB79" s="3">
+      <c r="BB79" s="4">
         <v>45110</v>
       </c>
     </row>
@@ -9635,8 +9645,8 @@
       <c r="C80" s="1">
         <v>2</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>269</v>
+      <c r="D80" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>55</v>
@@ -9655,7 +9665,7 @@
         <v>59</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>61</v>
@@ -9681,22 +9691,22 @@
       </c>
       <c r="T80" s="1"/>
       <c r="U80" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="V80" s="1" t="s">
-        <v>271</v>
+        <v>258</v>
       </c>
       <c r="W80" s="1" t="s">
         <v>57</v>
       </c>
       <c r="X80" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y80" s="1">
         <v>13</v>
       </c>
       <c r="Z80" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AA80" s="1" t="s">
         <v>57</v>
@@ -9723,7 +9733,7 @@
         <v>57</v>
       </c>
       <c r="AI80" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="AJ80" s="1" t="s">
         <v>59</v>
@@ -9767,7 +9777,7 @@
       <c r="BA80" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB80" s="3">
+      <c r="BB80" s="4">
         <v>45110</v>
       </c>
     </row>
@@ -9781,8 +9791,8 @@
       <c r="C81" s="1">
         <v>2</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>273</v>
+      <c r="D81" s="3" t="s">
+        <v>270</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>55</v>
@@ -9843,7 +9853,7 @@
     </row>
     <row r="82" spans="1:54">
       <c r="A82" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B82" s="1">
         <v>2021</v>
@@ -9851,8 +9861,8 @@
       <c r="C82" s="1">
         <v>4</v>
       </c>
-      <c r="D82" s="2" t="s">
-        <v>275</v>
+      <c r="D82" s="3" t="s">
+        <v>272</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>163</v>
@@ -9873,7 +9883,7 @@
         <v>59</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="L82" s="1" t="s">
         <v>61</v>
@@ -9902,7 +9912,7 @@
         <v>57</v>
       </c>
       <c r="V82" s="1" t="s">
-        <v>277</v>
+        <v>81</v>
       </c>
       <c r="W82" s="1" t="s">
         <v>59</v>
@@ -9961,7 +9971,7 @@
         <v>57</v>
       </c>
       <c r="AQ82" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="AR82" s="1" t="s">
         <v>59</v>
@@ -9970,8 +9980,8 @@
       <c r="AT82" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU82" s="5" t="s">
-        <v>279</v>
+      <c r="AU82" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="AV82" s="1" t="s">
         <v>72</v>
@@ -9987,13 +9997,13 @@
       <c r="BA82" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB82" s="3">
+      <c r="BB82" s="4">
         <v>45141</v>
       </c>
     </row>
     <row r="83" spans="1:54">
       <c r="A83" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B83" s="1">
         <v>2022</v>
@@ -10001,8 +10011,8 @@
       <c r="C83" s="1">
         <v>1</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>280</v>
+      <c r="D83" s="13" t="s">
+        <v>276</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>163</v>
@@ -10017,8 +10027,12 @@
         <v>1</v>
       </c>
       <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
+      <c r="J83" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K83" s="1" t="s">
+        <v>295</v>
+      </c>
       <c r="L83" s="1" t="s">
         <v>61</v>
       </c>
@@ -10058,7 +10072,7 @@
         <v>3</v>
       </c>
       <c r="Z83" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="AA83" s="1" t="s">
         <v>57</v>
@@ -10085,14 +10099,14 @@
         <v>57</v>
       </c>
       <c r="AI83" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="AJ83" s="1" t="s">
         <v>59</v>
       </c>
       <c r="AK83" s="1"/>
       <c r="AL83" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="AM83" s="1" t="s">
         <v>59</v>
@@ -10117,7 +10131,7 @@
         <v>82</v>
       </c>
       <c r="AU83" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="AV83" s="1"/>
       <c r="AW83" s="1" t="s">
@@ -10131,13 +10145,13 @@
       <c r="BA83" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB83" s="3">
+      <c r="BB83" s="4">
         <v>45141</v>
       </c>
     </row>
     <row r="84" spans="1:54">
       <c r="A84" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B84" s="1">
         <v>2021</v>
@@ -10145,8 +10159,8 @@
       <c r="C84" s="1">
         <v>4</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>285</v>
+      <c r="D84" s="3" t="s">
+        <v>281</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>163</v>
@@ -10167,7 +10181,7 @@
         <v>59</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>61</v>
@@ -10208,7 +10222,7 @@
         <v>1</v>
       </c>
       <c r="Z84" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="AA84" s="1" t="s">
         <v>57</v>
@@ -10235,7 +10249,7 @@
         <v>57</v>
       </c>
       <c r="AI84" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="AJ84" s="1" t="s">
         <v>57</v>
@@ -10266,8 +10280,8 @@
       <c r="AT84" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU84" s="5" t="s">
-        <v>288</v>
+      <c r="AU84" s="6" t="s">
+        <v>284</v>
       </c>
       <c r="AV84" s="1" t="s">
         <v>72</v>
@@ -10283,13 +10297,13 @@
       <c r="BA84" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="BB84" s="3">
+      <c r="BB84" s="4">
         <v>45141</v>
       </c>
     </row>
     <row r="85" spans="1:54">
       <c r="A85" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B85" s="1">
         <v>2022</v>
@@ -10297,8 +10311,8 @@
       <c r="C85" s="1">
         <v>5</v>
       </c>
-      <c r="D85" s="5" t="s">
-        <v>289</v>
+      <c r="D85" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>163</v>
@@ -10317,7 +10331,7 @@
         <v>59</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>61</v>
@@ -10345,16 +10359,20 @@
       <c r="U85" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="V85" s="1"/>
+      <c r="V85" s="1">
+        <v>1</v>
+      </c>
       <c r="W85" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="X85" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="X85" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="Y85" s="1">
         <v>1</v>
       </c>
       <c r="Z85" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AA85" s="1" t="s">
         <v>57</v>
@@ -10385,7 +10403,7 @@
         <v>57</v>
       </c>
       <c r="AK85" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="AL85" s="1" t="s">
         <v>68</v>
@@ -10403,7 +10421,7 @@
         <v>57</v>
       </c>
       <c r="AQ85" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="AR85" s="1" t="s">
         <v>59</v>
@@ -10422,18 +10440,18 @@
       </c>
       <c r="AY85" s="1"/>
       <c r="AZ85" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="BA85" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="BB85" s="3">
+      <c r="BB85" s="4">
         <v>45141</v>
       </c>
     </row>
     <row r="86" spans="1:54">
       <c r="A86" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B86" s="1">
         <v>2022</v>
@@ -10441,8 +10459,8 @@
       <c r="C86" s="1">
         <v>2</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>294</v>
+      <c r="D86" s="6" t="s">
+        <v>290</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>163</v>
@@ -10460,7 +10478,9 @@
       <c r="J86" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K86" s="1"/>
+      <c r="K86" s="1" t="s">
+        <v>296</v>
+      </c>
       <c r="L86" s="1" t="s">
         <v>78</v>
       </c>
@@ -10494,7 +10514,7 @@
         <v>57</v>
       </c>
       <c r="X86" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y86" s="1">
         <v>1</v>
@@ -10527,13 +10547,13 @@
         <v>57</v>
       </c>
       <c r="AI86" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AJ86" s="1" t="s">
         <v>59</v>
       </c>
       <c r="AK86" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AL86" s="1" t="s">
         <v>68</v>
@@ -10560,8 +10580,8 @@
       <c r="AT86" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AU86" s="2" t="s">
-        <v>297</v>
+      <c r="AU86" s="3" t="s">
+        <v>293</v>
       </c>
       <c r="AV86" s="1" t="s">
         <v>72</v>
@@ -10577,13 +10597,13 @@
       <c r="BA86" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BB86" s="3">
+      <c r="BB86" s="4">
         <v>45141</v>
       </c>
     </row>
     <row r="87" spans="1:54">
       <c r="A87" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B87" s="1">
         <v>2022</v>
@@ -10591,8 +10611,8 @@
       <c r="C87" s="1">
         <v>2</v>
       </c>
-      <c r="D87" s="2" t="s">
-        <v>298</v>
+      <c r="D87" s="3" t="s">
+        <v>294</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>163</v>
@@ -10617,7 +10637,6 @@
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
       <c r="U87" s="1"/>
-      <c r="V87" s="1"/>
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
       <c r="Y87" s="1"/>
@@ -70809,7 +70828,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="BA2:BA1161" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"great,medium,poor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U2:U75 U77:U79 J2:J1161 M2:M1161 S2:S1161 U81:U1161 W2:W1161 AA2:AH1161 AJ2:AJ1161 AM2:AP1161 AR2:AR1161" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="U2:U75 U77:U79 J2:J1161 M2:M1161 S2:S1161 U81:U1161 W2:W1161 AA2:AH1161 AJ2:AJ1161 AM2:AP1161 AR2:AR1161 V82" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"yes,no,unclear"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="X2:X1161" xr:uid="{00000000-0002-0000-0000-000005000000}">

</xml_diff>